<commit_message>
add top search bar using autocomplete
</commit_message>
<xml_diff>
--- a/public/index.xlsx
+++ b/public/index.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wallacelee/Documents/aws-course/Projects/engagement/nextui-engage/nextui-engage/public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E915C016-02A2-7647-A1FF-36510D505453}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA0109B-B273-F248-9B2E-55249506CF34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15660" yWindow="1360" windowWidth="24040" windowHeight="19120" xr2:uid="{FB60AA26-AAED-4D4A-941A-35A5A885384F}"/>
+    <workbookView xWindow="15200" yWindow="560" windowWidth="24040" windowHeight="19120" xr2:uid="{FB60AA26-AAED-4D4A-941A-35A5A885384F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="52">
   <si>
     <t>Platform</t>
   </si>
@@ -93,10 +93,6 @@
   </si>
   <si>
     <t>Clone [EMTOOLS-8]</t>
-  </si>
-  <si>
-    <t>http://localhost/l/cp/zreH1pni
-Note: Day2 configuration for OneAgent deployment</t>
   </si>
   <si>
     <t>Change Management Zone settings
@@ -192,7 +188,33 @@
 Non-Production onboarding must be completed first. Applications should be validated and internally self-signed off. It is recommended to let the application run in the Non-Production environment for 1-2 weeks before proceeding with the Production environment onboarding.</t>
   </si>
   <si>
-    <t>This deployment involves using a Golden Image to deploy a Linux server with the Dynatrace OneAgent pre-installed. It is designed specifically for newly built Linux servers whose Environment and OS identifiers (8th-9th characters of the server build ID) match one of the following configurations:
+    <t>Virtual Machine</t>
+  </si>
+  <si>
+    <t>Create Jira ticket|https://example.com/post-deployment</t>
+  </si>
+  <si>
+    <t>Please create a Jira ticket to enable monitoring for your virtual machine in Dynatrace
+Jira ticket|url</t>
+  </si>
+  <si>
+    <t>AWS Service</t>
+  </si>
+  <si>
+    <t>Infrastructure Baseline Recommended Metrics and Thresholds|https://example.com/post-deployment</t>
+  </si>
+  <si>
+    <t>Metrics for AWS service are available by default in CloudWatch. You can find the baseline, recommended metrics and threshold in the reference link below.</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>How to verify Windows Servers base monitoring in SCOM|https://example.com/post-deployment
+SCOM Base Monitoring|https://example.com/post-deployment</t>
+  </si>
+  <si>
+    <t>This deployment involves using a Golden Image to deploy a Linux server to your on-prem environment with the Dynatrace OneAgent pre-installed for base monitoring. It is designed specifically for newly built Linux servers whose Environment and OS identifiers (8th-9th characters of the server build ID) match one of the following configurations:
 ·             pl - (PR)Prod Linux
 ·             fl - (PF)Perf Linux
 ·             sl - (DV)SIT Linux
@@ -201,30 +223,7 @@
 E.g.'xxx.xxx.xxx' server has an Environment and OS identifier of 'lq'</t>
   </si>
   <si>
-    <t>Virtual Machine</t>
-  </si>
-  <si>
-    <t>Create Jira ticket|https://example.com/post-deployment</t>
-  </si>
-  <si>
-    <t>Please create a Jira ticket to enable monitoring for your virtual machine in Dynatrace
-Jira ticket|url</t>
-  </si>
-  <si>
-    <t>AWS Service</t>
-  </si>
-  <si>
-    <t>Infrastructure Baseline Recommended Metrics and Thresholds|https://example.com/post-deployment</t>
-  </si>
-  <si>
-    <t>Metrics for AWS service are available by default in CloudWatch. You can find the baseline, recommended metrics and threshold in the reference link below.</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>How to verify Windows Servers base monitoring in SCOM|https://example.com/post-deployment
-SCOM Base Monitoring|https://example.com/post-deployment</t>
+    <t>Note: Day2 configuration for OneAgent deployment</t>
   </si>
 </sst>
 </file>
@@ -275,7 +274,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -286,17 +285,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -636,8 +638,8 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F4" sqref="F4"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -666,7 +668,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>8</v>
@@ -675,7 +677,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="204" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="221" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -689,13 +691,13 @@
         <v>6</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="187" x14ac:dyDescent="0.2">
@@ -715,10 +717,10 @@
         <v>15</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="136" x14ac:dyDescent="0.2">
@@ -738,13 +740,13 @@
         <v>12</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="51" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1</v>
       </c>
@@ -760,8 +762,8 @@
       <c r="E5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>19</v>
+      <c r="F5" s="8" t="s">
+        <v>51</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>13</v>
@@ -784,7 +786,7 @@
         <v>17</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>18</v>
@@ -798,7 +800,7 @@
         <v>14</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>14</v>
@@ -806,9 +808,11 @@
       <c r="E7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="G7" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="119" x14ac:dyDescent="0.2">
@@ -819,19 +823,19 @@
         <v>14</v>
       </c>
       <c r="C8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="51" x14ac:dyDescent="0.2">
@@ -842,7 +846,7 @@
         <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>14</v>
@@ -850,8 +854,11 @@
       <c r="E9" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="F9" s="6" t="s">
+        <v>48</v>
+      </c>
       <c r="G9" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="255" x14ac:dyDescent="0.2">
@@ -862,19 +869,19 @@
         <v>14</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="68" x14ac:dyDescent="0.2">
@@ -885,7 +892,7 @@
         <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>14</v>
@@ -894,41 +901,41 @@
         <v>17</v>
       </c>
       <c r="F11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="E12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>49</v>
-      </c>
       <c r="G12" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>9</v>
@@ -940,18 +947,18 @@
         <v>17</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>3</v>
@@ -963,22 +970,21 @@
         <v>17</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G6" r:id="rId1" display="http://localhost/browse/EMTOOLS-8" xr:uid="{B11E77FA-C187-8642-A91D-9DE22E4467AD}"/>
     <hyperlink ref="G5" r:id="rId2" display="http://localhost/sp?id=sc_cat_item&amp;sys_id=232017a287499118f55f646d8bbb3566&amp;sysparm_category=c9b18bfa87dd7d10f74e646d8bbb3523" xr:uid="{B39A02F8-5541-414B-A7CB-87D318ED4782}"/>
-    <hyperlink ref="F5" r:id="rId3" xr:uid="{990F0EAC-27BD-9840-9672-1DB4025FDB55}"/>
-    <hyperlink ref="G7" r:id="rId4" display="http://localhost/sp?id=sc_cat_item&amp;sys_id=3b99a4b4db152cd0f55f400e0b961963&amp;sysparm_category=f14b02901b2ad89433d7766ecc4bcb68&amp;catalog_id=-1" xr:uid="{C36C89DB-C2BF-3E42-864E-3E458A49D805}"/>
-    <hyperlink ref="G8" r:id="rId5" display="C:/wiki/spaces/EMTOOLS/pages/548518762/Dynatrace+Infrastructure+to+Full+Stack+Monitoring+User+Guide" xr:uid="{65390177-80B4-A04E-98B5-002209638189}"/>
-    <hyperlink ref="G9" r:id="rId6" display="https://bmogc.service-now.com/sp?id=sc_cat_item&amp;sys_id=3b99a4b4db152cd0f55f400e0b961963&amp;sysparm_category=f14b02901b2ad89433d7766ecc4bcb68&amp;catalog_id=-1" xr:uid="{6F966F6C-2342-9349-B5FA-8C1C2933424F}"/>
-    <hyperlink ref="G11" r:id="rId7" xr:uid="{42F25980-2FA1-D146-9620-8D0FA0E2D354}"/>
-    <hyperlink ref="G10" r:id="rId8" display="C:/wiki/spaces/EMTH/pages/571375638/Infrastructure+Base+Monitoring+Thresholds" xr:uid="{8D02913F-5A47-A642-BFB1-D8F481BBBDB7}"/>
+    <hyperlink ref="G7" r:id="rId3" display="http://localhost/sp?id=sc_cat_item&amp;sys_id=3b99a4b4db152cd0f55f400e0b961963&amp;sysparm_category=f14b02901b2ad89433d7766ecc4bcb68&amp;catalog_id=-1" xr:uid="{C36C89DB-C2BF-3E42-864E-3E458A49D805}"/>
+    <hyperlink ref="G8" r:id="rId4" display="C:/wiki/spaces/EMTOOLS/pages/548518762/Dynatrace+Infrastructure+to+Full+Stack+Monitoring+User+Guide" xr:uid="{65390177-80B4-A04E-98B5-002209638189}"/>
+    <hyperlink ref="G9" r:id="rId5" display="https://bmogc.service-now.com/sp?id=sc_cat_item&amp;sys_id=3b99a4b4db152cd0f55f400e0b961963&amp;sysparm_category=f14b02901b2ad89433d7766ecc4bcb68&amp;catalog_id=-1" xr:uid="{6F966F6C-2342-9349-B5FA-8C1C2933424F}"/>
+    <hyperlink ref="G11" r:id="rId6" xr:uid="{42F25980-2FA1-D146-9620-8D0FA0E2D354}"/>
+    <hyperlink ref="G10" r:id="rId7" display="C:/wiki/spaces/EMTH/pages/571375638/Infrastructure+Base+Monitoring+Thresholds" xr:uid="{8D02913F-5A47-A642-BFB1-D8F481BBBDB7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>